<commit_message>
feat: Spring MVC 的 @ControllerAdvice 之 ResponseBodyAdvice 返回值增强笔记
</commit_message>
<xml_diff>
--- a/02-后端框架/05-SpringMVC/attachments-SpringMVC/01-SpringMVC基础-相关表格.xlsx
+++ b/02-后端框架/05-SpringMVC/attachments-SpringMVC/01-SpringMVC基础-相关表格.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DispatcherServlet 委托处理接口" sheetId="14" r:id="rId1"/>
     <sheet name="控制方法参数绑定类型" sheetId="15" r:id="rId2"/>
     <sheet name="控制方法返回值类型" sheetId="16" r:id="rId3"/>
+    <sheet name="相关实现" sheetId="18" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="140">
   <si>
     <t>------------</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1791,6 +1792,799 @@
   </si>
   <si>
     <t>返回值会通过`HttpMessageConverter`实现转换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MessageConverter</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> instances from the HTTP request and response. By default, this converter supports all text media types (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>text/*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>) and writes with a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>Content-Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>text/plain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>FormHttpMessageConverter</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write form data from the HTTP request and response. By default, this converter reads and writes the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>application/x-www-form-urlencoded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> media type. Form data is read from and written into a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>MultiValueMap&lt;String, String&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>. The converter can also write (but not read) multipart data read from a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>MultiValueMap&lt;String, Object&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>. By default, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>multipart/form-data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> is supported. As of Spring Framework 5.2, additional multipart subtypes can be supported for writing form data. Consult the javadoc for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>FormHttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> for further details.</t>
+    </r>
+  </si>
+  <si>
+    <t>ByteArrayHttpMessageConverter</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write byte arrays from the HTTP request and response. By default, this converter supports all media types (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>*/*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>) and writes with a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>Content-Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>application/octet-stream</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>. You can override this by setting the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>supportedMediaTypes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> property and overriding </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>getContentType(byte[])</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write XML by using Spring’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>Marshaller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>Unmarshaller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> abstractions from the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>org.springframework.oxm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> package. This converter requires a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>Marshaller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>Unmarshaller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> before it can be used. You can inject these through constructor or bean properties. By default, this converter supports </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>text/xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>application/xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>SourceHttpMessageConverter</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>javax.xml.transform.Source</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> from the HTTP request and response. Only </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>DOMSource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>SAXSource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>, and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>StreamSource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> are supported. By default, this converter supports </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>text/xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>application/xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>BufferedImageHttpMessageConverter</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>java.awt.image.BufferedImage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> from the HTTP request and response. This converter reads and writes the media type supported by the Java I/O API.</t>
+    </r>
+  </si>
+  <si>
+    <t>MessageConverter 实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StringHttpMessageConverter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MarshallingHttpMessageConverter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MappingJackson2HttpMessageConverter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`MappingJackson2HttpMessageConverter`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MappingJackson2XmlHttpMessageConverter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`MappingJackson2XmlHttpMessageConverter`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>HttpMessageConverter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> implementation that can read and write JSON by using Jackson’s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectMapper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>. You can customize JSON mapping as needed through the use of Jackson’s provided annotations. When you need further control (for cases where custom JSON serializers/deserializers need to be provided for specific types), you can inject a custom </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectMapper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> through the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>ObjectMapper</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t> property. By default, this converter supports </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monaco"/>
+        <family val="3"/>
+      </rPr>
+      <t>application/json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>An HttpMessageConverter implementation that can read and write XML by using Jackson XML extension’s XmlMapper. You can customize XML mapping as needed through the use of JAXB or Jackson’s provided annotations. When you need further control (for cases where custom XML serializers/deserializers need to be provided for specific types), you can inject a custom XmlMapper through the ObjectMapper property. By default, this converter supports application/xml.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过使用Jackson XML扩展的`XmlMapper`读写XML格式数据，默认支持HTTP的application/xml</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过使用Jackson的`ObjectMapper`来读写JSON格式数据，默认支持HTTP的application/json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1798,7 +2592,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1847,19 +2641,26 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Vollkorn"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF3502"/>
-      <name val="Source Code Pro"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1878,8 +2679,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1902,11 +2715,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD4DFDF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD4DFDF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD4DFDF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD4DFDF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD4DFDF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD4DFDF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD4DFDF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD4DFDF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD4DFDF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD4DFDF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD4DFDF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD4DFDF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1946,6 +2811,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2817,7 +3700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3025,7 +3908,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="31.5">
+    <row r="26" spans="2:3" ht="30.75">
       <c r="B26" s="10" t="s">
         <v>98</v>
       </c>
@@ -3049,7 +3932,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="31.5">
+    <row r="29" spans="2:3" ht="30.75">
       <c r="B29" s="12" t="s">
         <v>104</v>
       </c>
@@ -3057,7 +3940,279 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="78.75">
+    <row r="30" spans="2:3" ht="77.25">
+      <c r="B30" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15">
+      <c r="B31" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="100.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="4"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>$F$1&amp;B2&amp;$F$1&amp;C2&amp;$F$1</f>
+        <v>|MessageConverter 实现|说明|</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f t="shared" ref="E3:E10" si="0">$F$1&amp;B3&amp;$F$1&amp;C3&amp;$F$1</f>
+        <v>|:------------:|------------|</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="27">
+      <c r="B4" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|`MappingJackson2HttpMessageConverter`|通过使用Jackson的`ObjectMapper`来读写JSON格式数据，默认支持HTTP的application/json|</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="27">
+      <c r="B5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|`MappingJackson2XmlHttpMessageConverter`|通过使用Jackson XML扩展的`XmlMapper`读写XML格式数据，默认支持HTTP的application/xml|</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="E6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|||</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="E7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|||</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="E8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|||</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|||</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="E10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>|||</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:6" ht="14.25" thickBot="1"/>
+    <row r="15" spans="2:6" ht="16.5" thickBot="1">
+      <c r="B15" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="35.25" thickBot="1">
+      <c r="B16" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="101.25" thickBot="1">
+      <c r="B17" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="52.5" thickBot="1">
+      <c r="B18" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="66.75" thickBot="1">
+      <c r="B19" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="63.75" thickBot="1">
+      <c r="B20" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="33.75" thickBot="1">
+      <c r="B21" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="52.5" thickBot="1">
+      <c r="B22" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="33.75" thickBot="1">
+      <c r="B23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="30.75">
+      <c r="B25" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="30.75">
+      <c r="B26" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="72">
+      <c r="B27" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="31.5">
+      <c r="B28" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="30.75">
+      <c r="B29" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="77.25">
       <c r="B30" s="11" t="s">
         <v>106</v>
       </c>

</xml_diff>